<commit_message>
Alle grafieken staan erin
</commit_message>
<xml_diff>
--- a/Dashboard_Caro/Data/Monthly Tesla Vehicle Sales.xlsx
+++ b/Dashboard_Caro/Data/Monthly Tesla Vehicle Sales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroh\OneDrive - Universiteit Hasselt\2020-2021\Business intelligence\Project\BUSIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroh\OneDrive - Universiteit Hasselt\2020-2021\Business intelligence\Project\BUSIN\Dashboard_Caro\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2FD586-299E-4777-A252-5D6C36775206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEAAF65-25EF-4012-B742-5FD660CAE06E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A7E820A4-D284-4ACE-A8E8-3BC0C4C0F32F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>April</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>October</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -430,7 +427,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,18 +665,6 @@
       <c r="I6">
         <v>7215</v>
       </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>